<commit_message>
adds code for South East London
</commit_message>
<xml_diff>
--- a/data/reference/tlhc_project_name_lookup.xlsx
+++ b/data/reference/tlhc_project_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_targeted_lung_health_check/mi_data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C48BB00-6D47-4D08-B509-55B5CE03AF4F}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C862E483-0953-46BD-9DF2-366367725B84}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30630" yWindow="1620" windowWidth="28515" windowHeight="16035" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
+    <workbookView xWindow="19020" yWindow="4320" windowWidth="24465" windowHeight="10620" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="project_names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
   <si>
     <t>calc_submitting_organisation_name</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>NMS00</t>
+  </si>
+  <si>
+    <t>Barnsley Bassetlaw Rotherham</t>
+  </si>
+  <si>
+    <t>South East London</t>
+  </si>
+  <si>
+    <t>72Q00</t>
   </si>
 </sst>
 </file>
@@ -303,8 +312,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G30" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G30" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G31" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G31" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
     <sortCondition ref="A1:A29"/>
   </sortState>
@@ -618,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CD548A-BDC3-4DC3-B9AC-AB8BA5F6EB3E}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1109,9 +1118,23 @@
         <v>53</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes name of Luton to 'Luton South Bedfordshire' and sets NK LDCT data to not split by CCG
</commit_message>
<xml_diff>
--- a/data/reference/tlhc_project_name_lookup.xlsx
+++ b/data/reference/tlhc_project_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{008B6F64-2177-4F1D-A4A5-26029744F2EC}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E86E682D-C70E-48A6-A130-C5170AE598A5}"/>
   <bookViews>
-    <workbookView xWindow="31350" yWindow="1050" windowWidth="24330" windowHeight="14340" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="26040" windowHeight="17445" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="project_names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
   <si>
     <t>calc_submitting_organisation_name</t>
   </si>
@@ -158,18 +158,12 @@
     <t>Cheshire and Merseyside</t>
   </si>
   <si>
-    <t>Luton</t>
-  </si>
-  <si>
     <t>Smoking provider</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>LDCT provider  - shared between Bradford &amp; North Kirklees</t>
-  </si>
-  <si>
     <t>project_name_place</t>
   </si>
   <si>
@@ -222,6 +216,9 @@
   </si>
   <si>
     <t>72Q00</t>
+  </si>
+  <si>
+    <t>08/03/2023 No longer need splitting - they're uploading separate submissions. LDCT provider  - shared between Bradford &amp; North Kirklees.</t>
   </si>
 </sst>
 </file>
@@ -630,7 +627,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>
@@ -661,10 +658,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -675,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -689,10 +686,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,10 +700,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -714,13 +711,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -728,13 +725,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -742,13 +739,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,13 +809,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,16 +865,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -902,7 +899,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -913,7 +910,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
@@ -936,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -967,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,8 +977,8 @@
       <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1">
-        <v>1</v>
+      <c r="D23" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
@@ -990,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,8 +1000,8 @@
       <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="1">
-        <v>1</v>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
@@ -1013,7 +1010,7 @@
         <v>6</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1026,8 +1023,8 @@
       <c r="C25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="1">
-        <v>1</v>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>25</v>
@@ -1036,7 +1033,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,7 +1075,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1087,7 +1084,7 @@
         <v>36</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1098,7 +1095,7 @@
         <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1107,35 +1104,35 @@
         <v>37</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds Barnsley's organisational code
</commit_message>
<xml_diff>
--- a/data/reference/tlhc_project_name_lookup.xlsx
+++ b/data/reference/tlhc_project_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E86E682D-C70E-48A6-A130-C5170AE598A5}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA864BBD-8ACB-4306-9479-7A54AB1C0FDB}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="26040" windowHeight="17445" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
+    <workbookView xWindow="5460" yWindow="5460" windowWidth="27990" windowHeight="15735" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="project_names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>calc_submitting_organisation_name</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>08/03/2023 No longer need splitting - they're uploading separate submissions. LDCT provider  - shared between Bradford &amp; North Kirklees.</t>
+  </si>
+  <si>
+    <t>Barnsley</t>
+  </si>
+  <si>
+    <t>02P00</t>
   </si>
 </sst>
 </file>
@@ -309,8 +315,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G31" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G31" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G32" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
     <sortCondition ref="A1:A29"/>
   </sortState>
@@ -624,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CD548A-BDC3-4DC3-B9AC-AB8BA5F6EB3E}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,6 +1141,20 @@
         <v>49</v>
       </c>
     </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adds new record for Doncaster's new provider
</commit_message>
<xml_diff>
--- a/data/reference/tlhc_project_name_lookup.xlsx
+++ b/data/reference/tlhc_project_name_lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhs-my.sharepoint.com/personal/craig_parylo2_nhs_net/Documents/Documents/Projects/610_tlhc/data/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA864BBD-8ACB-4306-9479-7A54AB1C0FDB}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{45606466-144E-4C9B-BF1C-AC0E1F64E427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA2B79CD-9C9B-4247-B3E6-4BDC1FD6038C}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="5460" windowWidth="27990" windowHeight="15735" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
+    <workbookView xWindow="105" yWindow="45" windowWidth="22215" windowHeight="13545" xr2:uid="{06DEEB60-F1E9-4E46-BD67-412DE133CE47}"/>
   </bookViews>
   <sheets>
     <sheet name="project_names" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t>calc_submitting_organisation_name</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>02P00</t>
+  </si>
+  <si>
+    <t>A9N8Z</t>
+  </si>
+  <si>
+    <t>New TLHC provider</t>
   </si>
 </sst>
 </file>
@@ -315,10 +321,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G32" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
-    <sortCondition ref="A1:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}" name="Table1" displayName="Table1" ref="A1:G33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G33" xr:uid="{5B982C70-7A37-4BA6-923E-37A5E76C24B4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D30">
+    <sortCondition ref="A1:A30"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{8343DF0D-781A-4D3C-8FD4-91F8F4DE5F5C}" name="calc_submitting_organisation_name" dataDxfId="6"/>
@@ -334,9 +340,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -374,7 +380,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -480,7 +486,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -622,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CD548A-BDC3-4DC3-B9AC-AB8BA5F6EB3E}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,27 +846,33 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -871,41 +883,41 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>40</v>
+      <c r="D16" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -913,13 +925,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -930,7 +942,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
@@ -938,39 +950,36 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,22 +987,16 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>6</v>
+      <c r="D23" s="1">
+        <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,7 +1013,7 @@
         <v>49</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>6</v>
@@ -1033,10 +1036,10 @@
         <v>49</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>60</v>
@@ -1044,53 +1047,56 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1107,35 +1113,41 @@
         <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>49</v>
@@ -1143,15 +1155,29 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>